<commit_message>
going to host in pythonanywhere
</commit_message>
<xml_diff>
--- a/home/data/faq.xlsx
+++ b/home/data/faq.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="418">
   <si>
     <t>Question</t>
   </si>
@@ -1281,21 +1281,6 @@
   </si>
   <si>
     <t>jose</t>
-  </si>
-  <si>
-    <t>vanam</t>
-  </si>
-  <si>
-    <t>Aloshi</t>
-  </si>
-  <si>
-    <t>peduvanam</t>
-  </si>
-  <si>
-    <t>shonu</t>
-  </si>
-  <si>
-    <t>kundan</t>
   </si>
 </sst>
 </file>
@@ -2257,10 +2242,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C197"/>
+  <dimension ref="A1:C195"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="C197" sqref="C197"/>
+      <selection activeCell="C195" sqref="C195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="2"/>
@@ -4404,37 +4389,9 @@
         <v>416</v>
       </c>
     </row>
-    <row r="195" spans="1:3">
+    <row r="195" spans="1:1">
       <c r="A195" t="s">
         <v>417</v>
-      </c>
-      <c r="B195" t="s">
-        <v>418</v>
-      </c>
-      <c r="C195" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3">
-      <c r="A196" t="s">
-        <v>419</v>
-      </c>
-      <c r="B196" t="s">
-        <v>420</v>
-      </c>
-      <c r="C196" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3">
-      <c r="A197" t="s">
-        <v>421</v>
-      </c>
-      <c r="B197" t="s">
-        <v>422</v>
-      </c>
-      <c r="C197" t="s">
-        <v>416</v>
       </c>
     </row>
   </sheetData>

</xml_diff>